<commit_message>
2 mögliche Varianten zur übermittlung der Daten bei der Matrix. Auswahl muss noch getroffen werden.
</commit_message>
<xml_diff>
--- a/Schnittstelle_intern/Schnittstellenprotokoll UART.xlsx
+++ b/Schnittstelle_intern/Schnittstellenprotokoll UART.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remow\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remow\Documents\LedCube\Schnittstelle_intern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F0A761-A026-42A2-ABBD-997AEFF07A62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB032222-59DC-49E5-84E8-EC7B21A3F32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{477071D6-9D88-409A-80F4-D2274AE8481A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Funktion</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>mit ganzer layer angezündet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Beispiel</t>
+  </si>
+  <si>
+    <t>0x8912345678</t>
+  </si>
+  <si>
+    <t>0x89 0x12345678</t>
+  </si>
+  <si>
+    <t>Variante 2:</t>
+  </si>
+  <si>
+    <t>Variante 1:</t>
+  </si>
+  <si>
+    <t>Var1 oder Var2?</t>
   </si>
 </sst>
 </file>
@@ -546,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E789E199-D552-403E-A76F-7F888702C81D}">
-  <dimension ref="B2:L17"/>
+  <dimension ref="B2:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -558,16 +579,18 @@
     <col min="4" max="4" width="11.86328125" customWidth="1"/>
     <col min="5" max="5" width="11.953125" customWidth="1"/>
     <col min="12" max="12" width="12.2265625" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -584,12 +607,12 @@
         <v>38400</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -600,7 +623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -611,7 +634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -622,7 +645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -633,7 +656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -644,7 +667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -655,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -666,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -677,7 +700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -688,7 +711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -702,7 +725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.75">
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
@@ -730,8 +753,11 @@
       <c r="L16" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="N16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.75">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -764,6 +790,28 @@
       </c>
       <c r="L17" t="s">
         <v>38</v>
+      </c>
+      <c r="M17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" t="s">
+        <v>50</v>
+      </c>
+      <c r="O17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="N18" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="N19" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>